<commit_message>
Updated data inputs and broke checks
</commit_message>
<xml_diff>
--- a/data-raw/model-inputs/targets.xlsx
+++ b/data-raw/model-inputs/targets.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lffox/Dropbox (Grattan Institute)/Transport Program/Project - Electric vehicles/Analysis/efficiency-standards-analysis/cba-standards/cba-standards/data/model-inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lffox/Dropbox (Grattan Institute)/Transport Program/Project - Electric vehicles/Analysis/fleeteffSim/data-raw/model-inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F25CFA-285E-E240-A190-5CC1E7FDA8FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA79721-600D-374C-A6F0-34FC67D092B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21020" xr2:uid="{8B27FF0C-4EF2-3749-AB9A-861A4F7E9CE0}"/>
   </bookViews>
@@ -61,24 +61,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>year</t>
   </si>
   <si>
-    <t>mild_s</t>
+    <t>target_linear</t>
   </si>
   <si>
-    <t>agressive_s</t>
+    <t>target_ambitious</t>
   </si>
   <si>
-    <t>three-phase</t>
-  </si>
-  <si>
-    <t>linear_2023</t>
-  </si>
-  <si>
-    <t>two_phase_aggressive</t>
+    <t>target_central</t>
   </si>
 </sst>
 </file>
@@ -213,7 +207,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>linear_2023</c:v>
+                  <c:v>target_linear</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -354,7 +348,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>two_phase_aggressive</c:v>
+                  <c:v>target_ambitious</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -495,7 +489,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>three-phase</c:v>
+                  <c:v>target_central</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1760,35 +1754,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C52943D3-D443-1C46-B8C5-1FA463E1C284}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2020</v>
       </c>
@@ -1801,14 +1789,8 @@
       <c r="D2">
         <v>181.6</v>
       </c>
-      <c r="E2">
-        <v>181.6</v>
-      </c>
-      <c r="F2">
-        <v>181.6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2021</v>
       </c>
@@ -1821,14 +1803,8 @@
       <c r="D3" s="2">
         <v>180</v>
       </c>
-      <c r="E3">
-        <v>180</v>
-      </c>
-      <c r="F3">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2022</v>
       </c>
@@ -1841,14 +1817,8 @@
       <c r="D4" s="2">
         <v>180</v>
       </c>
-      <c r="E4">
-        <v>178</v>
-      </c>
-      <c r="F4">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2023</v>
       </c>
@@ -1863,14 +1833,8 @@
       <c r="D5" s="2">
         <v>170</v>
       </c>
-      <c r="E5">
-        <v>174</v>
-      </c>
-      <c r="F5">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2024</v>
       </c>
@@ -1885,14 +1849,8 @@
       <c r="D6" s="2">
         <v>160</v>
       </c>
-      <c r="E6">
-        <v>169</v>
-      </c>
-      <c r="F6">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2025</v>
       </c>
@@ -1907,14 +1865,8 @@
       <c r="D7" s="2">
         <v>150</v>
       </c>
-      <c r="E7">
-        <v>160</v>
-      </c>
-      <c r="F7">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2026</v>
       </c>
@@ -1930,14 +1882,8 @@
         <f>D7-25</f>
         <v>125</v>
       </c>
-      <c r="E8">
-        <v>140</v>
-      </c>
-      <c r="F8">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2027</v>
       </c>
@@ -1953,14 +1899,8 @@
         <f t="shared" ref="D9:D11" si="2">D8-25</f>
         <v>100</v>
       </c>
-      <c r="E9">
-        <v>120</v>
-      </c>
-      <c r="F9">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2028</v>
       </c>
@@ -1976,14 +1916,8 @@
         <f t="shared" si="2"/>
         <v>75</v>
       </c>
-      <c r="E10">
-        <v>87</v>
-      </c>
-      <c r="F10">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2029</v>
       </c>
@@ -1999,14 +1933,8 @@
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="E11">
-        <v>55</v>
-      </c>
-      <c r="F11">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2030</v>
       </c>
@@ -2020,14 +1948,8 @@
       <c r="D12" s="3">
         <v>25</v>
       </c>
-      <c r="E12">
-        <v>33</v>
-      </c>
-      <c r="F12">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2031</v>
       </c>
@@ -2043,14 +1965,8 @@
         <f>D12-5</f>
         <v>20</v>
       </c>
-      <c r="E13">
-        <v>22</v>
-      </c>
-      <c r="F13">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2032</v>
       </c>
@@ -2066,14 +1982,8 @@
         <f t="shared" ref="D14:D17" si="4">D13-5</f>
         <v>15</v>
       </c>
-      <c r="E14">
-        <v>15</v>
-      </c>
-      <c r="F14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2033</v>
       </c>
@@ -2089,14 +1999,8 @@
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="E15">
-        <v>9</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2034</v>
       </c>
@@ -2112,14 +2016,8 @@
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="E16">
-        <v>4</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2035</v>
       </c>
@@ -2134,14 +2032,8 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2036</v>
       </c>
@@ -2154,14 +2046,8 @@
       <c r="D18">
         <v>0</v>
       </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2037</v>
       </c>
@@ -2174,14 +2060,8 @@
       <c r="D19">
         <v>0</v>
       </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2038</v>
       </c>
@@ -2194,14 +2074,8 @@
       <c r="D20">
         <v>0</v>
       </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2039</v>
       </c>
@@ -2214,14 +2088,8 @@
       <c r="D21">
         <v>0</v>
       </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2040</v>
       </c>
@@ -2234,14 +2102,8 @@
       <c r="D22">
         <v>0</v>
       </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2041</v>
       </c>
@@ -2254,14 +2116,8 @@
       <c r="D23">
         <v>0</v>
       </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2042</v>
       </c>
@@ -2274,14 +2130,8 @@
       <c r="D24">
         <v>0</v>
       </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2043</v>
       </c>
@@ -2294,14 +2144,8 @@
       <c r="D25">
         <v>0</v>
       </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2044</v>
       </c>
@@ -2314,14 +2158,8 @@
       <c r="D26">
         <v>0</v>
       </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2045</v>
       </c>
@@ -2334,14 +2172,8 @@
       <c r="D27">
         <v>0</v>
       </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2046</v>
       </c>
@@ -2354,14 +2186,8 @@
       <c r="D28">
         <v>0</v>
       </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2047</v>
       </c>
@@ -2374,14 +2200,8 @@
       <c r="D29">
         <v>0</v>
       </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2048</v>
       </c>
@@ -2394,14 +2214,8 @@
       <c r="D30">
         <v>0</v>
       </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2049</v>
       </c>
@@ -2414,14 +2228,8 @@
       <c r="D31">
         <v>0</v>
       </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2050</v>
       </c>
@@ -2432,12 +2240,6 @@
         <v>0</v>
       </c>
       <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32">
         <v>0</v>
       </c>
     </row>

</xml_diff>